<commit_message>
Make Nifti_output right size
</commit_message>
<xml_diff>
--- a/AncillaryFiles/AllinOne_Gas_Exchange_Summary.xlsx
+++ b/AncillaryFiles/AllinOne_Gas_Exchange_Summary.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="146">
   <si>
     <t>Subject</t>
   </si>
@@ -442,6 +442,15 @@
   </si>
   <si>
     <t>RBC2Barrier_Bin6_Percent</t>
+  </si>
+  <si>
+    <t>Xe-027</t>
+  </si>
+  <si>
+    <t>2021-11-05</t>
+  </si>
+  <si>
+    <t>2021-11-15</t>
   </si>
 </sst>
 </file>
@@ -462,7 +471,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -473,15 +482,19 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -491,7 +504,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BN3"/>
+  <dimension ref="A1:BN4"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="7.7109375" customWidth="true"/>
@@ -507,7 +520,7 @@
     <col min="11" max="11" width="13.42578125" customWidth="true"/>
     <col min="12" max="12" width="17.28515625" customWidth="true"/>
     <col min="13" max="13" width="11.7109375" customWidth="true"/>
-    <col min="14" max="14" width="12.42578125" customWidth="true"/>
+    <col min="14" max="14" width="13.42578125" customWidth="true"/>
     <col min="15" max="15" width="13.42578125" customWidth="true"/>
     <col min="16" max="16" width="11.7109375" customWidth="true"/>
     <col min="17" max="17" width="17.140625" customWidth="true"/>
@@ -563,603 +576,803 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AA1" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AB1" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AC1" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AD1" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AE1" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AF1" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AG1" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AH1" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AI1" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AJ1" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AK1" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AL1" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AM1" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AN1" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AO1" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AP1" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AQ1" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AR1" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AS1" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AT1" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AU1" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AV1" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AW1" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AX1" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="AY1" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="AZ1" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BA1" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BB1" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BC1" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BD1" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BE1" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BF1" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BG1" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BH1" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BI1" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BJ1" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BK1" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="BL1" s="1" t="s">
+      <c r="BL1" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="BM1" s="1" t="s">
+      <c r="BM1" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="BN1" s="1" t="s">
+      <c r="BN1" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="0">
+      <c r="C2">
         <v>0.45000000000000001</v>
       </c>
-      <c r="D2" s="0">
+      <c r="D2">
         <v>14.6</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="G2" s="0">
+      <c r="G2">
         <v>-7404.8168495507389</v>
       </c>
-      <c r="H2" s="0">
+      <c r="H2">
         <v>-676.06295798337976</v>
       </c>
-      <c r="I2" s="0">
+      <c r="I2">
         <v>19.839965161695176</v>
       </c>
-      <c r="J2" s="0">
+      <c r="J2">
         <v>8.4778950020438568</v>
       </c>
-      <c r="K2" s="0">
+      <c r="K2">
         <v>1.6343103789497482</v>
       </c>
-      <c r="L2" s="0">
+      <c r="L2">
         <v>1.0160384881866751</v>
       </c>
-      <c r="M2" s="0">
+      <c r="M2">
         <v>1.202070435134841</v>
       </c>
-      <c r="N2" s="0">
+      <c r="N2">
         <v>-1.3551241806464991</v>
       </c>
-      <c r="O2" s="0">
+      <c r="O2">
         <v>83.698222818808574</v>
       </c>
-      <c r="P2" s="0">
+      <c r="P2">
         <v>173.51425092476322</v>
       </c>
-      <c r="Q2" s="0">
+      <c r="Q2">
         <v>0.45564516799623056</v>
       </c>
-      <c r="R2" s="0">
+      <c r="R2">
         <v>1.9039582735829244</v>
       </c>
-      <c r="S2" s="0">
+      <c r="S2">
         <v>60.144245517376163</v>
       </c>
-      <c r="T2" s="0">
+      <c r="T2">
         <v>38.047928072998737</v>
       </c>
-      <c r="U2" s="0">
+      <c r="U2">
         <v>83.899802160220005</v>
       </c>
-      <c r="V2" s="0">
+      <c r="V2">
         <v>47.870544934888045</v>
       </c>
-      <c r="W2" s="0">
+      <c r="W2">
         <v>29.886688947824446</v>
       </c>
-      <c r="X2" s="0">
+      <c r="X2">
         <v>13.948522512766598</v>
       </c>
-      <c r="Y2" s="0">
+      <c r="Y2">
         <v>0.51826332443391454</v>
       </c>
-      <c r="Z2" s="0">
+      <c r="Z2">
         <v>0.19509785555195366</v>
       </c>
-      <c r="AA2" s="0">
+      <c r="AA2">
         <v>0.8192096256583139</v>
       </c>
-      <c r="AB2" s="0">
+      <c r="AB2">
         <v>0.16673385688213496</v>
       </c>
-      <c r="AC2" s="0">
+      <c r="AC2">
         <v>0.71946738912806274</v>
       </c>
-      <c r="AD2" s="0">
+      <c r="AD2">
         <v>0.15803349662667318</v>
       </c>
-      <c r="AE2" s="0">
+      <c r="AE2">
         <v>0.36149409761978657</v>
       </c>
-      <c r="AF2" s="0">
+      <c r="AF2">
         <v>0.13614474898312848</v>
       </c>
-      <c r="AG2" s="0">
+      <c r="AG2">
         <v>0.51725386056609235</v>
       </c>
-      <c r="AH2" s="0">
+      <c r="AH2">
         <v>0.21079016916715887</v>
       </c>
-      <c r="AI2" s="0">
+      <c r="AI2">
         <v>1.3099721630915342</v>
       </c>
-      <c r="AJ2" s="0">
+      <c r="AJ2">
         <v>6.3288030129359756</v>
       </c>
-      <c r="AK2" s="0">
+      <c r="AK2">
         <v>20.754871458981498</v>
       </c>
-      <c r="AL2" s="0">
+      <c r="AL2">
         <v>42.222040281644013</v>
       </c>
-      <c r="AM2" s="0">
+      <c r="AM2">
         <v>25.356148681840512</v>
       </c>
-      <c r="AN2" s="0">
+      <c r="AN2">
         <v>4.0281644015064675</v>
       </c>
-      <c r="AO2" s="0">
+      <c r="AO2">
         <v>0.92915214866434381</v>
       </c>
-      <c r="AP2" s="0">
+      <c r="AP2">
         <v>15.637962502074002</v>
       </c>
-      <c r="AQ2" s="0">
+      <c r="AQ2">
         <v>50.199104031856642</v>
       </c>
-      <c r="AR2" s="0">
+      <c r="AR2">
         <v>31.707317073170731</v>
       </c>
-      <c r="AS2" s="0">
+      <c r="AS2">
         <v>1.4186162269785962</v>
       </c>
-      <c r="AT2" s="0">
+      <c r="AT2">
         <v>0.10784801725568277</v>
       </c>
-      <c r="AU2" s="0">
+      <c r="AU2">
         <v>0.21569603451136554</v>
       </c>
-      <c r="AV2" s="0">
+      <c r="AV2">
         <v>12.369337979094077</v>
       </c>
-      <c r="AW2" s="0">
+      <c r="AW2">
         <v>46.449311431889825</v>
       </c>
-      <c r="AX2" s="0">
+      <c r="AX2">
         <v>38.053758088601292</v>
       </c>
-      <c r="AY2" s="0">
+      <c r="AY2">
         <v>2.7044964327194294</v>
       </c>
-      <c r="AZ2" s="0">
+      <c r="AZ2">
         <v>0.19080803052928488</v>
       </c>
-      <c r="BA2" s="0">
+      <c r="BA2">
         <v>0</v>
       </c>
-      <c r="BB2" s="0">
+      <c r="BB2">
         <v>0.016592002654720425</v>
       </c>
-      <c r="BC2" s="0">
+      <c r="BC2">
         <v>1.4186162269785962</v>
       </c>
-      <c r="BD2" s="0">
+      <c r="BD2">
         <v>12.86709805873569</v>
       </c>
-      <c r="BE2" s="0">
+      <c r="BE2">
         <v>53.177368508378962</v>
       </c>
-      <c r="BF2" s="0">
+      <c r="BF2">
         <v>31.433549029367846</v>
       </c>
-      <c r="BG2" s="0">
+      <c r="BG2">
         <v>1.0287041645926662</v>
       </c>
-      <c r="BH2" s="0">
+      <c r="BH2">
         <v>0.074664011946241921</v>
       </c>
-      <c r="BI2" s="0">
+      <c r="BI2">
         <v>1.3439522150323544</v>
       </c>
-      <c r="BJ2" s="0">
+      <c r="BJ2">
         <v>8.9596814335490294</v>
       </c>
-      <c r="BK2" s="0">
+      <c r="BK2">
         <v>46.938775510204081</v>
       </c>
-      <c r="BL2" s="0">
+      <c r="BL2">
         <v>40.584038493446158</v>
       </c>
-      <c r="BM2" s="0">
+      <c r="BM2">
         <v>2.1237763398042144</v>
       </c>
-      <c r="BN2" s="0">
+      <c r="BN2">
         <v>0.049776007964161276</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="0">
+      <c r="C3">
         <v>0.46000000000000002</v>
       </c>
-      <c r="D3" s="0">
+      <c r="D3">
         <v>14.6</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="G3" s="0">
+      <c r="G3">
         <v>-7399.5508136481785</v>
       </c>
-      <c r="H3" s="0">
+      <c r="H3">
         <v>-663.50499056099898</v>
       </c>
-      <c r="I3" s="0">
+      <c r="I3">
         <v>-2.37681536188565</v>
       </c>
-      <c r="J3" s="0">
+      <c r="J3">
         <v>10.587963723713139</v>
       </c>
-      <c r="K3" s="0">
+      <c r="K3">
         <v>1.6487240815240689</v>
       </c>
-      <c r="L3" s="0">
+      <c r="L3">
         <v>1.0034857799787291</v>
       </c>
-      <c r="M3" s="0">
+      <c r="M3">
         <v>1.2789145352643261</v>
       </c>
-      <c r="N3" s="0">
+      <c r="N3">
         <v>-0.16182632727921875</v>
       </c>
-      <c r="O3" s="0">
+      <c r="O3">
         <v>82.920941786685361</v>
       </c>
-      <c r="P3" s="0">
+      <c r="P3">
         <v>170.70285579709673</v>
       </c>
-      <c r="Q3" s="0">
+      <c r="Q3">
         <v>0.29769310194742193</v>
       </c>
-      <c r="R3" s="0">
+      <c r="R3">
         <v>0.10473203887072051</v>
       </c>
-      <c r="S3" s="0">
+      <c r="S3">
         <v>104.38056844404132</v>
       </c>
-      <c r="T3" s="0">
+      <c r="T3">
         <v>36.276401676210433</v>
       </c>
-      <c r="U3" s="0">
+      <c r="U3">
         <v>81.641605811590068</v>
       </c>
-      <c r="V3" s="0">
+      <c r="V3">
         <v>42.009497632182587</v>
       </c>
-      <c r="W3" s="0">
+      <c r="W3">
         <v>28.307730429635022</v>
       </c>
-      <c r="X3" s="0">
+      <c r="X3">
         <v>8.1916895107065102</v>
       </c>
-      <c r="Y3" s="0">
+      <c r="Y3">
         <v>0.4308943443532387</v>
       </c>
-      <c r="Z3" s="0">
+      <c r="Z3">
         <v>0.23045464703951873</v>
       </c>
-      <c r="AA3" s="0">
+      <c r="AA3">
         <v>0.68146062543641017</v>
       </c>
-      <c r="AB3" s="0">
+      <c r="AB3">
         <v>0.17918253143404514</v>
       </c>
-      <c r="AC3" s="0">
+      <c r="AC3">
         <v>0.63692791229671353</v>
       </c>
-      <c r="AD3" s="0">
+      <c r="AD3">
         <v>0.16557923795379881</v>
       </c>
-      <c r="AE3" s="0">
+      <c r="AE3">
         <v>0.20586513772977383</v>
       </c>
-      <c r="AF3" s="0">
+      <c r="AF3">
         <v>0.12135941831562774</v>
       </c>
-      <c r="AG3" s="0">
+      <c r="AG3">
         <v>0.33389084781247574</v>
       </c>
-      <c r="AH3" s="0">
+      <c r="AH3">
         <v>0.17964083758251878</v>
       </c>
-      <c r="AI3" s="0">
+      <c r="AI3">
         <v>8.9372280919825986</v>
       </c>
-      <c r="AJ3" s="0">
+      <c r="AJ3">
         <v>11.870727159726538</v>
       </c>
-      <c r="AK3" s="0">
+      <c r="AK3">
         <v>25.456805469235551</v>
       </c>
-      <c r="AL3" s="0">
+      <c r="AL3">
         <v>33.312616532007461</v>
       </c>
-      <c r="AM3" s="0">
+      <c r="AM3">
         <v>16.768178993163456</v>
       </c>
-      <c r="AN3" s="0">
+      <c r="AN3">
         <v>3.6544437538844003</v>
       </c>
-      <c r="AO3" s="0">
+      <c r="AO3">
         <v>4.2042042042042045</v>
       </c>
-      <c r="AP3" s="0">
+      <c r="AP3">
         <v>40.090090090090094</v>
       </c>
-      <c r="AQ3" s="0">
+      <c r="AQ3">
         <v>48.55309855309855</v>
       </c>
-      <c r="AR3" s="0">
+      <c r="AR3">
         <v>6.6748566748566747</v>
       </c>
-      <c r="AS3" s="0">
+      <c r="AS3">
         <v>0.4095004095004095</v>
       </c>
-      <c r="AT3" s="0">
+      <c r="AT3">
         <v>0.068250068250068255</v>
       </c>
-      <c r="AU3" s="0">
+      <c r="AU3">
         <v>1.0237510237510237</v>
       </c>
-      <c r="AV3" s="0">
+      <c r="AV3">
         <v>21.198471198471196</v>
       </c>
-      <c r="AW3" s="0">
+      <c r="AW3">
         <v>62.052962052962059</v>
       </c>
-      <c r="AX3" s="0">
+      <c r="AX3">
         <v>14.196014196014195</v>
       </c>
-      <c r="AY3" s="0">
+      <c r="AY3">
         <v>1.4332514332514332</v>
       </c>
-      <c r="AZ3" s="0">
+      <c r="AZ3">
         <v>0.040950040950040956</v>
       </c>
-      <c r="BA3" s="0">
+      <c r="BA3">
         <v>0.013650013650013651</v>
       </c>
-      <c r="BB3" s="0">
+      <c r="BB3">
         <v>0.040950040950040956</v>
       </c>
-      <c r="BC3" s="0">
+      <c r="BC3">
         <v>10.455910455910455</v>
       </c>
-      <c r="BD3" s="0">
+      <c r="BD3">
         <v>45.140595140595138</v>
       </c>
-      <c r="BE3" s="0">
+      <c r="BE3">
         <v>41.632541632541631</v>
       </c>
-      <c r="BF3" s="0">
+      <c r="BF3">
         <v>2.6890526890526889</v>
       </c>
-      <c r="BG3" s="0">
+      <c r="BG3">
         <v>0.040950040950040956</v>
       </c>
-      <c r="BH3" s="0">
+      <c r="BH3">
         <v>0.040950040950040956</v>
       </c>
-      <c r="BI3" s="0">
+      <c r="BI3">
         <v>10.346710346710347</v>
       </c>
-      <c r="BJ3" s="0">
+      <c r="BJ3">
         <v>25.716625716625718</v>
       </c>
-      <c r="BK3" s="0">
+      <c r="BK3">
         <v>54.818454818454818</v>
       </c>
-      <c r="BL3" s="0">
+      <c r="BL3">
         <v>8.5858585858585847</v>
       </c>
-      <c r="BM3" s="0">
+      <c r="BM3">
         <v>0.49140049140049141</v>
       </c>
-      <c r="BN3" s="0">
+      <c r="BN3">
         <v>0.040950040950040956</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C4">
+        <v>0.48999999999999999</v>
+      </c>
+      <c r="D4">
+        <v>14.6</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G4">
+        <v>-7413.9811910168964</v>
+      </c>
+      <c r="H4">
+        <v>-689.43170543902431</v>
+      </c>
+      <c r="I4">
+        <v>-25.454164450874018</v>
+      </c>
+      <c r="J4">
+        <v>4.8465931880155049</v>
+      </c>
+      <c r="K4">
+        <v>1.8667538048374819</v>
+      </c>
+      <c r="L4">
+        <v>1.032168969005067</v>
+      </c>
+      <c r="M4">
+        <v>1.3051358490613953</v>
+      </c>
+      <c r="N4">
+        <v>44.006803347171505</v>
+      </c>
+      <c r="O4">
+        <v>127.74624472800639</v>
+      </c>
+      <c r="P4">
+        <v>-130.68774753365457</v>
+      </c>
+      <c r="Q4">
+        <v>0.18002287079070675</v>
+      </c>
+      <c r="R4">
+        <v>3.0608304120380736</v>
+      </c>
+      <c r="S4">
+        <v>-32.614180595611344</v>
+      </c>
+      <c r="T4">
+        <v>28.041764156589107</v>
+      </c>
+      <c r="U4">
+        <v>63.917381532831357</v>
+      </c>
+      <c r="V4">
+        <v>46.672422502726917</v>
+      </c>
+      <c r="W4">
+        <v>32.800261948597289</v>
+      </c>
+      <c r="X4">
+        <v>5.2615345141325749</v>
+      </c>
+      <c r="Y4">
+        <v>0.32359462225804059</v>
+      </c>
+      <c r="Z4">
+        <v>0.22449877494338671</v>
+      </c>
+      <c r="AA4">
+        <v>0.80222847647790108</v>
+      </c>
+      <c r="AB4">
+        <v>0.19857102917410679</v>
+      </c>
+      <c r="AC4">
+        <v>0.77629811899367118</v>
+      </c>
+      <c r="AD4">
+        <v>0.19542806052750766</v>
+      </c>
+      <c r="AE4">
+        <v>0.14966051671901401</v>
+      </c>
+      <c r="AF4">
+        <v>0.095453613439439616</v>
+      </c>
+      <c r="AG4">
+        <v>0.20086434923734769</v>
+      </c>
+      <c r="AH4">
+        <v>0.12735989008503998</v>
+      </c>
+      <c r="AI4">
+        <v>15.906210392902409</v>
+      </c>
+      <c r="AJ4">
+        <v>22.042670046472328</v>
+      </c>
+      <c r="AK4">
+        <v>32.213772708069285</v>
+      </c>
+      <c r="AL4">
+        <v>19.254330376003377</v>
+      </c>
+      <c r="AM4">
+        <v>7.6573722010984362</v>
+      </c>
+      <c r="AN4">
+        <v>2.9256442754541614</v>
+      </c>
+      <c r="AO4">
+        <v>1.4066817382567194</v>
+      </c>
+      <c r="AP4">
+        <v>22.117558402411454</v>
+      </c>
+      <c r="AQ4">
+        <v>46.558653604621952</v>
+      </c>
+      <c r="AR4">
+        <v>26.161768399899522</v>
+      </c>
+      <c r="AS4">
+        <v>3.6799799045465966</v>
+      </c>
+      <c r="AT4">
+        <v>0.075357950263752832</v>
+      </c>
+      <c r="AU4">
+        <v>0.18839487565938207</v>
+      </c>
+      <c r="AV4">
+        <v>8.6159256468224061</v>
+      </c>
+      <c r="AW4">
+        <v>43.255463451394121</v>
+      </c>
+      <c r="AX4">
+        <v>36.171816126601357</v>
+      </c>
+      <c r="AY4">
+        <v>10.826425521225822</v>
+      </c>
+      <c r="AZ4">
+        <v>0.9294147199196181</v>
+      </c>
+      <c r="BA4">
+        <v>0.012559658377292136</v>
+      </c>
+      <c r="BB4">
+        <v>0</v>
+      </c>
+      <c r="BC4">
+        <v>24.215021351419242</v>
+      </c>
+      <c r="BD4">
+        <v>54.596834966088927</v>
+      </c>
+      <c r="BE4">
+        <v>19.881939211253457</v>
+      </c>
+      <c r="BF4">
+        <v>1.2434061793519218</v>
+      </c>
+      <c r="BG4">
+        <v>0.062798291886460689</v>
+      </c>
+      <c r="BH4">
+        <v>0</v>
+      </c>
+      <c r="BI4">
+        <v>29.125847776940468</v>
+      </c>
+      <c r="BJ4">
+        <v>45.541321276061289</v>
+      </c>
+      <c r="BK4">
+        <v>24.101984426023613</v>
+      </c>
+      <c r="BL4">
+        <v>1.1429289123335846</v>
+      </c>
+      <c r="BM4">
+        <v>0.087917608641044961</v>
+      </c>
+      <c r="BN4">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix orientation issues and app friendliness
</commit_message>
<xml_diff>
--- a/AncillaryFiles/AllinOne_Gas_Exchange_Summary.xlsx
+++ b/AncillaryFiles/AllinOne_Gas_Exchange_Summary.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="147">
   <si>
     <t>Subject</t>
   </si>
@@ -451,6 +451,9 @@
   </si>
   <si>
     <t>2021-11-15</t>
+  </si>
+  <si>
+    <t>2021-11-19</t>
   </si>
 </sst>
 </file>
@@ -471,7 +474,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -484,17 +487,25 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -504,7 +515,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BN4"/>
+  <dimension ref="A1:BN6"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="7.7109375" customWidth="true"/>
@@ -522,7 +533,7 @@
     <col min="13" max="13" width="11.7109375" customWidth="true"/>
     <col min="14" max="14" width="13.42578125" customWidth="true"/>
     <col min="15" max="15" width="13.42578125" customWidth="true"/>
-    <col min="16" max="16" width="11.7109375" customWidth="true"/>
+    <col min="16" max="16" width="12.42578125" customWidth="true"/>
     <col min="17" max="17" width="17.140625" customWidth="true"/>
     <col min="18" max="18" width="18.42578125" customWidth="true"/>
     <col min="19" max="19" width="17.7109375" customWidth="true"/>
@@ -576,210 +587,210 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="T1" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="U1" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="V1" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="W1" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="X1" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Y1" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="Z1" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AA1" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AB1" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AC1" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AD1" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AE1" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AF1" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AG1" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AH1" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AI1" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AJ1" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AK1" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="AL1" s="4" t="s">
+      <c r="AL1" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="AM1" s="4" t="s">
+      <c r="AM1" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="AN1" s="4" t="s">
+      <c r="AN1" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="AO1" s="4" t="s">
+      <c r="AO1" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="AP1" s="4" t="s">
+      <c r="AP1" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="AQ1" s="4" t="s">
+      <c r="AQ1" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="AR1" s="4" t="s">
+      <c r="AR1" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="AS1" s="4" t="s">
+      <c r="AS1" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="AT1" s="4" t="s">
+      <c r="AT1" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="AU1" s="4" t="s">
+      <c r="AU1" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="AV1" s="4" t="s">
+      <c r="AV1" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="AW1" s="4" t="s">
+      <c r="AW1" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="AX1" s="4" t="s">
+      <c r="AX1" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="AY1" s="4" t="s">
+      <c r="AY1" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="AZ1" s="4" t="s">
+      <c r="AZ1" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="BA1" s="4" t="s">
+      <c r="BA1" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="BB1" s="4" t="s">
+      <c r="BB1" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="BC1" s="4" t="s">
+      <c r="BC1" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="BD1" s="4" t="s">
+      <c r="BD1" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="BE1" s="4" t="s">
+      <c r="BE1" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="BF1" s="4" t="s">
+      <c r="BF1" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="BG1" s="4" t="s">
+      <c r="BG1" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="BH1" s="4" t="s">
+      <c r="BH1" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="BI1" s="4" t="s">
+      <c r="BI1" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="BJ1" s="4" t="s">
+      <c r="BJ1" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="BK1" s="4" t="s">
+      <c r="BK1" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="BL1" s="4" t="s">
+      <c r="BL1" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="BM1" s="4" t="s">
+      <c r="BM1" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="BN1" s="4" t="s">
+      <c r="BN1" s="8" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="8" t="s">
         <v>74</v>
       </c>
       <c r="C2">
@@ -788,10 +799,10 @@
       <c r="D2">
         <v>14.6</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="8" t="s">
         <v>82</v>
       </c>
       <c r="G2">
@@ -976,10 +987,10 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="8" t="s">
         <v>75</v>
       </c>
       <c r="C3">
@@ -988,10 +999,10 @@
       <c r="D3">
         <v>14.6</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="8" t="s">
         <v>82</v>
       </c>
       <c r="G3">
@@ -1176,10 +1187,10 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="8" t="s">
         <v>144</v>
       </c>
       <c r="C4">
@@ -1188,10 +1199,10 @@
       <c r="D4">
         <v>14.6</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="8" t="s">
         <v>82</v>
       </c>
       <c r="G4">
@@ -1373,6 +1384,406 @@
       </c>
       <c r="BN4">
         <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5">
+        <v>0.46000000000000002</v>
+      </c>
+      <c r="D5">
+        <v>14.6</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="G5">
+        <v>-7399.5510609391858</v>
+      </c>
+      <c r="H5">
+        <v>-663.52565132208792</v>
+      </c>
+      <c r="I5">
+        <v>-2.3745468730668358</v>
+      </c>
+      <c r="J5">
+        <v>10.587957922601987</v>
+      </c>
+      <c r="K5">
+        <v>1.6488518829155827</v>
+      </c>
+      <c r="L5">
+        <v>1.0034600165302596</v>
+      </c>
+      <c r="M5">
+        <v>1.2789117068403721</v>
+      </c>
+      <c r="N5">
+        <v>-0.16188560655732437</v>
+      </c>
+      <c r="O5">
+        <v>82.927229389685365</v>
+      </c>
+      <c r="P5">
+        <v>170.71287741585741</v>
+      </c>
+      <c r="Q5">
+        <v>0.29767026936348273</v>
+      </c>
+      <c r="R5">
+        <v>0.10475470466717995</v>
+      </c>
+      <c r="S5">
+        <v>105.28697933648426</v>
+      </c>
+      <c r="T5">
+        <v>36.639497232845422</v>
+      </c>
+      <c r="U5">
+        <v>83.009067352349163</v>
+      </c>
+      <c r="V5">
+        <v>42.014908816323285</v>
+      </c>
+      <c r="W5">
+        <v>28.283825254705842</v>
+      </c>
+      <c r="X5">
+        <v>8.1450858006302198</v>
+      </c>
+      <c r="Y5">
+        <v>0.42553056237505466</v>
+      </c>
+      <c r="Z5">
+        <v>0.23300773425490726</v>
+      </c>
+      <c r="AA5">
+        <v>0.68276174457409</v>
+      </c>
+      <c r="AB5">
+        <v>0.21774583292331645</v>
+      </c>
+      <c r="AC5">
+        <v>0.6377339981515634</v>
+      </c>
+      <c r="AD5">
+        <v>0.17700493332617426</v>
+      </c>
+      <c r="AE5">
+        <v>0.20570714326443451</v>
+      </c>
+      <c r="AF5">
+        <v>0.16870417576884322</v>
+      </c>
+      <c r="AG5">
+        <v>0.33176003454116748</v>
+      </c>
+      <c r="AH5">
+        <v>0.18317431032862019</v>
+      </c>
+      <c r="AI5">
+        <v>10.009671179883945</v>
+      </c>
+      <c r="AJ5">
+        <v>11.738394584139265</v>
+      </c>
+      <c r="AK5">
+        <v>25.386847195357831</v>
+      </c>
+      <c r="AL5">
+        <v>32.761121856866538</v>
+      </c>
+      <c r="AM5">
+        <v>16.477272727272727</v>
+      </c>
+      <c r="AN5">
+        <v>3.6266924564796903</v>
+      </c>
+      <c r="AO5">
+        <v>4.1644277270284791</v>
+      </c>
+      <c r="AP5">
+        <v>39.91133799032778</v>
+      </c>
+      <c r="AQ5">
+        <v>48.992477162815689</v>
+      </c>
+      <c r="AR5">
+        <v>6.4615797958087056</v>
+      </c>
+      <c r="AS5">
+        <v>0.38957549704459971</v>
+      </c>
+      <c r="AT5">
+        <v>0.080601826974744759</v>
+      </c>
+      <c r="AU5">
+        <v>0.99408919935518536</v>
+      </c>
+      <c r="AV5">
+        <v>21.010209564750134</v>
+      </c>
+      <c r="AW5">
+        <v>62.305212251477705</v>
+      </c>
+      <c r="AX5">
+        <v>14.212788823213327</v>
+      </c>
+      <c r="AY5">
+        <v>1.370231058570661</v>
+      </c>
+      <c r="AZ5">
+        <v>0.053734551316496508</v>
+      </c>
+      <c r="BA5">
+        <v>0</v>
+      </c>
+      <c r="BB5">
+        <v>0.053734551316496508</v>
+      </c>
+      <c r="BC5">
+        <v>11.055883933369156</v>
+      </c>
+      <c r="BD5">
+        <v>45.09672219236969</v>
+      </c>
+      <c r="BE5">
+        <v>41.026329930145081</v>
+      </c>
+      <c r="BF5">
+        <v>2.7001612036539493</v>
+      </c>
+      <c r="BG5">
+        <v>0.06716818914562063</v>
+      </c>
+      <c r="BH5">
+        <v>0.053734551316496508</v>
+      </c>
+      <c r="BI5">
+        <v>11.069317571198281</v>
+      </c>
+      <c r="BJ5">
+        <v>25.819451907576575</v>
+      </c>
+      <c r="BK5">
+        <v>54.083825900053739</v>
+      </c>
+      <c r="BL5">
+        <v>8.4497581945190756</v>
+      </c>
+      <c r="BM5">
+        <v>0.53734551316496504</v>
+      </c>
+      <c r="BN5">
+        <v>0.040300913487372379</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6">
+        <v>0.46000000000000002</v>
+      </c>
+      <c r="D6">
+        <v>14.6</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="G6">
+        <v>-7399.5510609391858</v>
+      </c>
+      <c r="H6">
+        <v>-663.52565132208792</v>
+      </c>
+      <c r="I6">
+        <v>-2.3745468730668358</v>
+      </c>
+      <c r="J6">
+        <v>10.587957922601987</v>
+      </c>
+      <c r="K6">
+        <v>1.6488518829155827</v>
+      </c>
+      <c r="L6">
+        <v>1.0034600165302596</v>
+      </c>
+      <c r="M6">
+        <v>1.2789117068403721</v>
+      </c>
+      <c r="N6">
+        <v>-0.16188560655732437</v>
+      </c>
+      <c r="O6">
+        <v>82.927229389685365</v>
+      </c>
+      <c r="P6">
+        <v>170.71287741585741</v>
+      </c>
+      <c r="Q6">
+        <v>0.29767026936348273</v>
+      </c>
+      <c r="R6">
+        <v>0.10475470466717995</v>
+      </c>
+      <c r="S6">
+        <v>105.28697933648426</v>
+      </c>
+      <c r="T6">
+        <v>36.639497232845422</v>
+      </c>
+      <c r="U6">
+        <v>83.009067352349163</v>
+      </c>
+      <c r="V6">
+        <v>42.014908816323285</v>
+      </c>
+      <c r="W6">
+        <v>28.283825254705842</v>
+      </c>
+      <c r="X6">
+        <v>8.1450858006302198</v>
+      </c>
+      <c r="Y6">
+        <v>0.42553056237505466</v>
+      </c>
+      <c r="Z6">
+        <v>0.23300773425490726</v>
+      </c>
+      <c r="AA6">
+        <v>0.68276174457409</v>
+      </c>
+      <c r="AB6">
+        <v>0.21774583292331645</v>
+      </c>
+      <c r="AC6">
+        <v>0.6377339981515634</v>
+      </c>
+      <c r="AD6">
+        <v>0.17700493332617426</v>
+      </c>
+      <c r="AE6">
+        <v>0.20570714326443451</v>
+      </c>
+      <c r="AF6">
+        <v>0.16870417576884322</v>
+      </c>
+      <c r="AG6">
+        <v>0.33176003454116748</v>
+      </c>
+      <c r="AH6">
+        <v>0.18317431032862019</v>
+      </c>
+      <c r="AI6">
+        <v>10.009671179883945</v>
+      </c>
+      <c r="AJ6">
+        <v>11.738394584139265</v>
+      </c>
+      <c r="AK6">
+        <v>25.386847195357831</v>
+      </c>
+      <c r="AL6">
+        <v>32.761121856866538</v>
+      </c>
+      <c r="AM6">
+        <v>16.477272727272727</v>
+      </c>
+      <c r="AN6">
+        <v>3.6266924564796903</v>
+      </c>
+      <c r="AO6">
+        <v>4.1644277270284791</v>
+      </c>
+      <c r="AP6">
+        <v>39.91133799032778</v>
+      </c>
+      <c r="AQ6">
+        <v>48.992477162815689</v>
+      </c>
+      <c r="AR6">
+        <v>6.4615797958087056</v>
+      </c>
+      <c r="AS6">
+        <v>0.38957549704459971</v>
+      </c>
+      <c r="AT6">
+        <v>0.080601826974744759</v>
+      </c>
+      <c r="AU6">
+        <v>0.99408919935518536</v>
+      </c>
+      <c r="AV6">
+        <v>21.010209564750134</v>
+      </c>
+      <c r="AW6">
+        <v>62.305212251477705</v>
+      </c>
+      <c r="AX6">
+        <v>14.212788823213327</v>
+      </c>
+      <c r="AY6">
+        <v>1.370231058570661</v>
+      </c>
+      <c r="AZ6">
+        <v>0.053734551316496508</v>
+      </c>
+      <c r="BA6">
+        <v>0</v>
+      </c>
+      <c r="BB6">
+        <v>0.053734551316496508</v>
+      </c>
+      <c r="BC6">
+        <v>11.055883933369156</v>
+      </c>
+      <c r="BD6">
+        <v>45.09672219236969</v>
+      </c>
+      <c r="BE6">
+        <v>41.026329930145081</v>
+      </c>
+      <c r="BF6">
+        <v>2.7001612036539493</v>
+      </c>
+      <c r="BG6">
+        <v>0.06716818914562063</v>
+      </c>
+      <c r="BH6">
+        <v>0.053734551316496508</v>
+      </c>
+      <c r="BI6">
+        <v>11.069317571198281</v>
+      </c>
+      <c r="BJ6">
+        <v>25.819451907576575</v>
+      </c>
+      <c r="BK6">
+        <v>54.083825900053739</v>
+      </c>
+      <c r="BL6">
+        <v>8.4497581945190756</v>
+      </c>
+      <c r="BM6">
+        <v>0.53734551316496504</v>
+      </c>
+      <c r="BN6">
+        <v>0.040300913487372379</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates for appended spectroscopy
</commit_message>
<xml_diff>
--- a/AncillaryFiles/AllinOne_Gas_Exchange_Summary.xlsx
+++ b/AncillaryFiles/AllinOne_Gas_Exchange_Summary.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="151">
   <si>
     <t>Subject</t>
   </si>
@@ -454,6 +454,18 @@
   </si>
   <si>
     <t>2021-11-19</t>
+  </si>
+  <si>
+    <t>Xe-037</t>
+  </si>
+  <si>
+    <t>2022-06-06</t>
+  </si>
+  <si>
+    <t>2022-06-17</t>
+  </si>
+  <si>
+    <t>20211119_HealthyCohort</t>
   </si>
 </sst>
 </file>
@@ -474,7 +486,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -491,11 +503,13 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -506,6 +520,8 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -519,29 +535,29 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="7.7109375" customWidth="true"/>
-    <col min="2" max="2" width="10.5703125" customWidth="true"/>
+    <col min="2" max="2" width="10.28515625" customWidth="true"/>
     <col min="3" max="3" width="5.140625" customWidth="true"/>
     <col min="4" max="4" width="10.5703125" customWidth="true"/>
     <col min="5" max="5" width="13" customWidth="true"/>
-    <col min="6" max="6" width="26.28515625" customWidth="true"/>
+    <col min="6" max="6" width="15" customWidth="true"/>
     <col min="7" max="7" width="14.5703125" customWidth="true"/>
     <col min="8" max="8" width="17.42578125" customWidth="true"/>
     <col min="9" max="9" width="14.85546875" customWidth="true"/>
-    <col min="10" max="10" width="11.7109375" customWidth="true"/>
+    <col min="10" max="10" width="10.5703125" customWidth="true"/>
     <col min="11" max="11" width="13.42578125" customWidth="true"/>
     <col min="12" max="12" width="17.28515625" customWidth="true"/>
-    <col min="13" max="13" width="11.7109375" customWidth="true"/>
-    <col min="14" max="14" width="13.42578125" customWidth="true"/>
+    <col min="13" max="13" width="10.85546875" customWidth="true"/>
+    <col min="14" max="14" width="10.5703125" customWidth="true"/>
     <col min="15" max="15" width="13.42578125" customWidth="true"/>
-    <col min="16" max="16" width="12.42578125" customWidth="true"/>
+    <col min="16" max="16" width="10.85546875" customWidth="true"/>
     <col min="17" max="17" width="17.140625" customWidth="true"/>
     <col min="18" max="18" width="18.42578125" customWidth="true"/>
     <col min="19" max="19" width="17.7109375" customWidth="true"/>
     <col min="20" max="20" width="15.7109375" customWidth="true"/>
-    <col min="21" max="21" width="11.7109375" customWidth="true"/>
+    <col min="21" max="21" width="8.85546875" customWidth="true"/>
     <col min="22" max="22" width="14.28515625" customWidth="true"/>
     <col min="23" max="23" width="11.7109375" customWidth="true"/>
-    <col min="24" max="24" width="11.7109375" customWidth="true"/>
+    <col min="24" max="24" width="9.140625" customWidth="true"/>
     <col min="25" max="25" width="17.140625" customWidth="true"/>
     <col min="26" max="26" width="19.42578125" customWidth="true"/>
     <col min="27" max="27" width="15.7109375" customWidth="true"/>
@@ -587,211 +603,211 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="O1" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="P1" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="Q1" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="R1" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="S1" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="T1" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="U1" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="V1" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="W1" s="8" t="s">
+      <c r="W1" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="X1" s="8" t="s">
+      <c r="X1" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="Y1" s="8" t="s">
+      <c r="Y1" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="Z1" s="8" t="s">
+      <c r="Z1" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="AA1" s="8" t="s">
+      <c r="AA1" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="AB1" s="8" t="s">
+      <c r="AB1" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="AC1" s="8" t="s">
+      <c r="AC1" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="AD1" s="8" t="s">
+      <c r="AD1" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="AE1" s="8" t="s">
+      <c r="AE1" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="AF1" s="8" t="s">
+      <c r="AF1" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="AG1" s="8" t="s">
+      <c r="AG1" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="AH1" s="8" t="s">
+      <c r="AH1" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="AI1" s="8" t="s">
+      <c r="AI1" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="AJ1" s="8" t="s">
+      <c r="AJ1" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="AK1" s="8" t="s">
+      <c r="AK1" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="AL1" s="8" t="s">
+      <c r="AL1" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="AM1" s="8" t="s">
+      <c r="AM1" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="AN1" s="8" t="s">
+      <c r="AN1" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="AO1" s="8" t="s">
+      <c r="AO1" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="AP1" s="8" t="s">
+      <c r="AP1" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="AQ1" s="8" t="s">
+      <c r="AQ1" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="AR1" s="8" t="s">
+      <c r="AR1" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="AS1" s="8" t="s">
+      <c r="AS1" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="AT1" s="8" t="s">
+      <c r="AT1" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="AU1" s="8" t="s">
+      <c r="AU1" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="AV1" s="8" t="s">
+      <c r="AV1" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="AW1" s="8" t="s">
+      <c r="AW1" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="AX1" s="8" t="s">
+      <c r="AX1" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="AY1" s="8" t="s">
+      <c r="AY1" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="AZ1" s="8" t="s">
+      <c r="AZ1" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="BA1" s="8" t="s">
+      <c r="BA1" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="BB1" s="8" t="s">
+      <c r="BB1" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="BC1" s="8" t="s">
+      <c r="BC1" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="BD1" s="8" t="s">
+      <c r="BD1" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="BE1" s="8" t="s">
+      <c r="BE1" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="BF1" s="8" t="s">
+      <c r="BF1" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="BG1" s="8" t="s">
+      <c r="BG1" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="BH1" s="8" t="s">
+      <c r="BH1" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="BI1" s="8" t="s">
+      <c r="BI1" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="BJ1" s="8" t="s">
+      <c r="BJ1" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="BK1" s="8" t="s">
+      <c r="BK1" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="BL1" s="8" t="s">
+      <c r="BL1" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="BM1" s="8" t="s">
+      <c r="BM1" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="BN1" s="8" t="s">
+      <c r="BN1" s="10" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>74</v>
+      <c r="A2" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>148</v>
       </c>
       <c r="C2">
         <v>0.45000000000000001</v>
@@ -799,191 +815,191 @@
       <c r="D2">
         <v>14.6</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>82</v>
+      <c r="E2" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>150</v>
       </c>
       <c r="G2">
-        <v>-7404.8168495507389</v>
+        <v>-7396.0699979126648</v>
       </c>
       <c r="H2">
-        <v>-676.06295798337976</v>
+        <v>-686.60554883478142</v>
       </c>
       <c r="I2">
-        <v>19.839965161695176</v>
+        <v>-0.21277834592285871</v>
       </c>
       <c r="J2">
-        <v>8.4778950020438568</v>
+        <v>12.452751020758702</v>
       </c>
       <c r="K2">
-        <v>1.6343103789497482</v>
+        <v>1.7535812844099699</v>
       </c>
       <c r="L2">
-        <v>1.0160384881866751</v>
+        <v>0.99421228726053779</v>
       </c>
       <c r="M2">
-        <v>1.202070435134841</v>
+        <v>1.2069861407667319</v>
       </c>
       <c r="N2">
-        <v>-1.3551241806464991</v>
+        <v>22.869523944135615</v>
       </c>
       <c r="O2">
-        <v>83.698222818808574</v>
+        <v>-162.64375004412031</v>
       </c>
       <c r="P2">
-        <v>173.51425092476322</v>
+        <v>-73.641403860233098</v>
       </c>
       <c r="Q2">
-        <v>0.45564516799623056</v>
+        <v>0.50422057628367611</v>
       </c>
       <c r="R2">
-        <v>1.9039582735829244</v>
+        <v>1.0824047123364617</v>
       </c>
       <c r="S2">
-        <v>60.144245517376163</v>
+        <v>116.16012608389605</v>
       </c>
       <c r="T2">
-        <v>38.047928072998737</v>
+        <v>18.763269575972821</v>
       </c>
       <c r="U2">
-        <v>83.899802160220005</v>
+        <v>42.522362885128132</v>
       </c>
       <c r="V2">
-        <v>47.870544934888045</v>
+        <v>40.173244040160888</v>
       </c>
       <c r="W2">
-        <v>29.886688947824446</v>
+        <v>24.592538019237868</v>
       </c>
       <c r="X2">
-        <v>13.948522512766598</v>
+        <v>12.565206315223557</v>
       </c>
       <c r="Y2">
-        <v>0.51826332443391454</v>
+        <v>0.58971121836490292</v>
       </c>
       <c r="Z2">
-        <v>0.19509785555195366</v>
+        <v>0.21720213227423599</v>
       </c>
       <c r="AA2">
-        <v>0.8192096256583139</v>
+        <v>0.96565968210125641</v>
       </c>
       <c r="AB2">
-        <v>0.16673385688213496</v>
+        <v>0.3059578572291124</v>
       </c>
       <c r="AC2">
-        <v>0.71946738912806274</v>
+        <v>0.83424191431792716</v>
       </c>
       <c r="AD2">
-        <v>0.15803349662667318</v>
+        <v>0.28127478092069452</v>
       </c>
       <c r="AE2">
-        <v>0.36149409761978657</v>
+        <v>0.46028858435511455</v>
       </c>
       <c r="AF2">
-        <v>0.13614474898312848</v>
+        <v>0.17206644731132772</v>
       </c>
       <c r="AG2">
-        <v>0.51725386056609235</v>
+        <v>0.56578582033089164</v>
       </c>
       <c r="AH2">
-        <v>0.21079016916715887</v>
+        <v>0.18373352569072537</v>
       </c>
       <c r="AI2">
-        <v>1.3099721630915342</v>
+        <v>2.8564916812276837</v>
       </c>
       <c r="AJ2">
-        <v>6.3288030129359756</v>
+        <v>5.5230570538631012</v>
       </c>
       <c r="AK2">
-        <v>20.754871458981498</v>
+        <v>17.997417002203147</v>
       </c>
       <c r="AL2">
-        <v>42.222040281644013</v>
+        <v>38.965281470789328</v>
       </c>
       <c r="AM2">
-        <v>25.356148681840512</v>
+        <v>31.056749981007371</v>
       </c>
       <c r="AN2">
-        <v>4.0281644015064675</v>
+        <v>3.601002810909367</v>
       </c>
       <c r="AO2">
-        <v>0.92915214866434381</v>
+        <v>0.6881989520606866</v>
       </c>
       <c r="AP2">
-        <v>15.637962502074002</v>
+        <v>10.581058887933056</v>
       </c>
       <c r="AQ2">
-        <v>50.199104031856642</v>
+        <v>33.189958551654023</v>
       </c>
       <c r="AR2">
-        <v>31.707317073170731</v>
+        <v>34.089309454915153</v>
       </c>
       <c r="AS2">
-        <v>1.4186162269785962</v>
+        <v>18.033940721044811</v>
       </c>
       <c r="AT2">
-        <v>0.10784801725568277</v>
+        <v>3.4175334323922733</v>
       </c>
       <c r="AU2">
-        <v>0.21569603451136554</v>
+        <v>0.20333150856338467</v>
       </c>
       <c r="AV2">
-        <v>12.369337979094077</v>
+        <v>8.0081332603425359</v>
       </c>
       <c r="AW2">
-        <v>46.449311431889825</v>
+        <v>38.539141315398453</v>
       </c>
       <c r="AX2">
-        <v>38.053758088601292</v>
+        <v>33.205599436928132</v>
       </c>
       <c r="AY2">
-        <v>2.7044964327194294</v>
+        <v>14.983968092594042</v>
       </c>
       <c r="AZ2">
-        <v>0.19080803052928488</v>
+        <v>4.3090638930163445</v>
       </c>
       <c r="BA2">
-        <v>0</v>
+        <v>0.54743098459372808</v>
       </c>
       <c r="BB2">
-        <v>0.016592002654720425</v>
+        <v>0.20333150856338467</v>
       </c>
       <c r="BC2">
-        <v>1.4186162269785962</v>
+        <v>0.84460780480175179</v>
       </c>
       <c r="BD2">
-        <v>12.86709805873569</v>
+        <v>7.6014702432157657</v>
       </c>
       <c r="BE2">
-        <v>53.177368508378962</v>
+        <v>29.00602174083053</v>
       </c>
       <c r="BF2">
-        <v>31.433549029367846</v>
+        <v>50.066473762414951</v>
       </c>
       <c r="BG2">
-        <v>1.0287041645926662</v>
+        <v>11.855791037772738</v>
       </c>
       <c r="BH2">
-        <v>0.074664011946241921</v>
+        <v>0.62563541096426056</v>
       </c>
       <c r="BI2">
-        <v>1.3439522150323544</v>
+        <v>0.71948072260889961</v>
       </c>
       <c r="BJ2">
-        <v>8.9596814335490294</v>
+        <v>5.0207241729881913</v>
       </c>
       <c r="BK2">
-        <v>46.938775510204081</v>
+        <v>34.034566356455777</v>
       </c>
       <c r="BL2">
-        <v>40.584038493446158</v>
+        <v>56.541800265895048</v>
       </c>
       <c r="BM2">
-        <v>2.1237763398042144</v>
+        <v>3.6443262688668181</v>
       </c>
       <c r="BN2">
-        <v>0.049776007964161276</v>
+        <v>0.039102213185266285</v>
       </c>
     </row>
     <row r="3">

</xml_diff>